<commit_message>
Mobile App translation logic
</commit_message>
<xml_diff>
--- a/Documents/ScreenLayouts/SCR-CMN-06-ChangePassword.xlsx
+++ b/Documents/ScreenLayouts/SCR-CMN-06-ChangePassword.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/ScreenLayouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315CA4DC-A4D0-0947-9BDB-9F1C885BF63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAEFBE0-F958-FB4C-9E87-C201C8C51650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
   <sheets>
     <sheet name="SCR-CMN-06" sheetId="5" r:id="rId1"/>
@@ -441,6 +441,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -468,32 +492,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1558,211 +1558,211 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43867302-6022-BC45-9802-796B2A9AA285}">
   <dimension ref="A1:DD76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="BP42" sqref="BP42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="BL34" sqref="BL34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2" defaultRowHeight="8" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
     </row>
     <row r="2" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
     </row>
     <row r="3" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="17"/>
-      <c r="AD3" s="17"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
+      <c r="AD3" s="25"/>
     </row>
     <row r="4" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="18" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18"/>
-      <c r="AD4" s="18"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="26"/>
     </row>
     <row r="5" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
     </row>
     <row r="6" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="18"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
     </row>
     <row r="9" spans="1:108" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
@@ -6118,998 +6118,998 @@
       <c r="CT60" s="11"/>
     </row>
     <row r="61" spans="3:98" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19" t="s">
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
-      <c r="M61" s="19"/>
-      <c r="N61" s="19"/>
-      <c r="O61" s="19"/>
-      <c r="P61" s="19"/>
-      <c r="Q61" s="19"/>
-      <c r="R61" s="19"/>
-      <c r="S61" s="19"/>
-      <c r="T61" s="19"/>
-      <c r="U61" s="19"/>
-      <c r="V61" s="19"/>
-      <c r="W61" s="19"/>
-      <c r="X61" s="19"/>
-      <c r="Y61" s="19" t="s">
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="27"/>
+      <c r="N61" s="27"/>
+      <c r="O61" s="27"/>
+      <c r="P61" s="27"/>
+      <c r="Q61" s="27"/>
+      <c r="R61" s="27"/>
+      <c r="S61" s="27"/>
+      <c r="T61" s="27"/>
+      <c r="U61" s="27"/>
+      <c r="V61" s="27"/>
+      <c r="W61" s="27"/>
+      <c r="X61" s="27"/>
+      <c r="Y61" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="Z61" s="19"/>
-      <c r="AA61" s="19"/>
-      <c r="AB61" s="19"/>
-      <c r="AC61" s="19"/>
-      <c r="AD61" s="19"/>
-      <c r="AE61" s="19"/>
-      <c r="AF61" s="19"/>
-      <c r="AG61" s="19"/>
-      <c r="AH61" s="19"/>
-      <c r="AI61" s="19"/>
-      <c r="AJ61" s="19"/>
-      <c r="AK61" s="19"/>
-      <c r="AL61" s="19"/>
-      <c r="AM61" s="19"/>
-      <c r="AN61" s="19" t="s">
+      <c r="Z61" s="27"/>
+      <c r="AA61" s="27"/>
+      <c r="AB61" s="27"/>
+      <c r="AC61" s="27"/>
+      <c r="AD61" s="27"/>
+      <c r="AE61" s="27"/>
+      <c r="AF61" s="27"/>
+      <c r="AG61" s="27"/>
+      <c r="AH61" s="27"/>
+      <c r="AI61" s="27"/>
+      <c r="AJ61" s="27"/>
+      <c r="AK61" s="27"/>
+      <c r="AL61" s="27"/>
+      <c r="AM61" s="27"/>
+      <c r="AN61" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AO61" s="19"/>
-      <c r="AP61" s="19"/>
-      <c r="AQ61" s="19"/>
-      <c r="AR61" s="19"/>
-      <c r="AS61" s="19"/>
-      <c r="AT61" s="19"/>
-      <c r="AU61" s="19"/>
-      <c r="AV61" s="19"/>
-      <c r="AW61" s="19"/>
-      <c r="AX61" s="19"/>
-      <c r="AY61" s="19"/>
-      <c r="AZ61" s="19"/>
-      <c r="BA61" s="19"/>
-      <c r="BB61" s="19"/>
-      <c r="BC61" s="19"/>
-      <c r="BD61" s="19"/>
-      <c r="BE61" s="19"/>
-      <c r="BF61" s="19"/>
-      <c r="BG61" s="19"/>
-      <c r="BH61" s="19"/>
-      <c r="BI61" s="19"/>
-      <c r="BJ61" s="19" t="s">
+      <c r="AO61" s="27"/>
+      <c r="AP61" s="27"/>
+      <c r="AQ61" s="27"/>
+      <c r="AR61" s="27"/>
+      <c r="AS61" s="27"/>
+      <c r="AT61" s="27"/>
+      <c r="AU61" s="27"/>
+      <c r="AV61" s="27"/>
+      <c r="AW61" s="27"/>
+      <c r="AX61" s="27"/>
+      <c r="AY61" s="27"/>
+      <c r="AZ61" s="27"/>
+      <c r="BA61" s="27"/>
+      <c r="BB61" s="27"/>
+      <c r="BC61" s="27"/>
+      <c r="BD61" s="27"/>
+      <c r="BE61" s="27"/>
+      <c r="BF61" s="27"/>
+      <c r="BG61" s="27"/>
+      <c r="BH61" s="27"/>
+      <c r="BI61" s="27"/>
+      <c r="BJ61" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="BK61" s="19"/>
-      <c r="BL61" s="19"/>
-      <c r="BM61" s="19"/>
-      <c r="BN61" s="19"/>
-      <c r="BO61" s="19"/>
-      <c r="BP61" s="19"/>
-      <c r="BQ61" s="19"/>
-      <c r="BR61" s="19"/>
-      <c r="BS61" s="19"/>
-      <c r="BT61" s="19"/>
-      <c r="BU61" s="19"/>
-      <c r="BV61" s="19"/>
-      <c r="BW61" s="19"/>
-      <c r="BX61" s="19"/>
-      <c r="BY61" s="19"/>
-      <c r="BZ61" s="19" t="s">
+      <c r="BK61" s="27"/>
+      <c r="BL61" s="27"/>
+      <c r="BM61" s="27"/>
+      <c r="BN61" s="27"/>
+      <c r="BO61" s="27"/>
+      <c r="BP61" s="27"/>
+      <c r="BQ61" s="27"/>
+      <c r="BR61" s="27"/>
+      <c r="BS61" s="27"/>
+      <c r="BT61" s="27"/>
+      <c r="BU61" s="27"/>
+      <c r="BV61" s="27"/>
+      <c r="BW61" s="27"/>
+      <c r="BX61" s="27"/>
+      <c r="BY61" s="27"/>
+      <c r="BZ61" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="CA61" s="19"/>
-      <c r="CB61" s="19"/>
-      <c r="CC61" s="19"/>
-      <c r="CD61" s="19"/>
-      <c r="CE61" s="19"/>
-      <c r="CF61" s="19"/>
-      <c r="CG61" s="19"/>
-      <c r="CH61" s="19"/>
-      <c r="CI61" s="19"/>
-      <c r="CJ61" s="19"/>
-      <c r="CK61" s="19"/>
-      <c r="CL61" s="19"/>
-      <c r="CM61" s="19"/>
-      <c r="CN61" s="19"/>
-      <c r="CO61" s="19"/>
-      <c r="CP61" s="19"/>
-      <c r="CQ61" s="19"/>
-      <c r="CR61" s="19"/>
-      <c r="CS61" s="19"/>
-      <c r="CT61" s="20"/>
+      <c r="CA61" s="27"/>
+      <c r="CB61" s="27"/>
+      <c r="CC61" s="27"/>
+      <c r="CD61" s="27"/>
+      <c r="CE61" s="27"/>
+      <c r="CF61" s="27"/>
+      <c r="CG61" s="27"/>
+      <c r="CH61" s="27"/>
+      <c r="CI61" s="27"/>
+      <c r="CJ61" s="27"/>
+      <c r="CK61" s="27"/>
+      <c r="CL61" s="27"/>
+      <c r="CM61" s="27"/>
+      <c r="CN61" s="27"/>
+      <c r="CO61" s="27"/>
+      <c r="CP61" s="27"/>
+      <c r="CQ61" s="27"/>
+      <c r="CR61" s="27"/>
+      <c r="CS61" s="27"/>
+      <c r="CT61" s="28"/>
     </row>
     <row r="62" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C62" s="26">
+      <c r="C62" s="30">
         <v>1</v>
       </c>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="13" t="s">
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="13"/>
-      <c r="O62" s="13"/>
-      <c r="P62" s="13"/>
-      <c r="Q62" s="13"/>
-      <c r="R62" s="13"/>
-      <c r="S62" s="13"/>
-      <c r="T62" s="13"/>
-      <c r="U62" s="13"/>
-      <c r="V62" s="13"/>
-      <c r="W62" s="13"/>
-      <c r="X62" s="13"/>
-      <c r="Y62" s="13" t="s">
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="21"/>
+      <c r="M62" s="21"/>
+      <c r="N62" s="21"/>
+      <c r="O62" s="21"/>
+      <c r="P62" s="21"/>
+      <c r="Q62" s="21"/>
+      <c r="R62" s="21"/>
+      <c r="S62" s="21"/>
+      <c r="T62" s="21"/>
+      <c r="U62" s="21"/>
+      <c r="V62" s="21"/>
+      <c r="W62" s="21"/>
+      <c r="X62" s="21"/>
+      <c r="Y62" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="Z62" s="13"/>
-      <c r="AA62" s="13"/>
-      <c r="AB62" s="13"/>
-      <c r="AC62" s="13"/>
-      <c r="AD62" s="13"/>
-      <c r="AE62" s="13"/>
-      <c r="AF62" s="13"/>
-      <c r="AG62" s="13"/>
-      <c r="AH62" s="13"/>
-      <c r="AI62" s="13"/>
-      <c r="AJ62" s="13"/>
-      <c r="AK62" s="13"/>
-      <c r="AL62" s="13"/>
-      <c r="AM62" s="13"/>
-      <c r="AN62" s="14" t="s">
+      <c r="Z62" s="21"/>
+      <c r="AA62" s="21"/>
+      <c r="AB62" s="21"/>
+      <c r="AC62" s="21"/>
+      <c r="AD62" s="21"/>
+      <c r="AE62" s="21"/>
+      <c r="AF62" s="21"/>
+      <c r="AG62" s="21"/>
+      <c r="AH62" s="21"/>
+      <c r="AI62" s="21"/>
+      <c r="AJ62" s="21"/>
+      <c r="AK62" s="21"/>
+      <c r="AL62" s="21"/>
+      <c r="AM62" s="21"/>
+      <c r="AN62" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AO62" s="14"/>
-      <c r="AP62" s="14"/>
-      <c r="AQ62" s="14"/>
-      <c r="AR62" s="14"/>
-      <c r="AS62" s="14"/>
-      <c r="AT62" s="14"/>
-      <c r="AU62" s="14"/>
-      <c r="AV62" s="14"/>
-      <c r="AW62" s="14"/>
-      <c r="AX62" s="14"/>
-      <c r="AY62" s="14"/>
-      <c r="AZ62" s="14"/>
-      <c r="BA62" s="14"/>
-      <c r="BB62" s="14"/>
-      <c r="BC62" s="14"/>
-      <c r="BD62" s="14"/>
-      <c r="BE62" s="14"/>
-      <c r="BF62" s="14"/>
-      <c r="BG62" s="14"/>
-      <c r="BH62" s="14"/>
-      <c r="BI62" s="14"/>
-      <c r="BJ62" s="13" t="s">
+      <c r="AO62" s="22"/>
+      <c r="AP62" s="22"/>
+      <c r="AQ62" s="22"/>
+      <c r="AR62" s="22"/>
+      <c r="AS62" s="22"/>
+      <c r="AT62" s="22"/>
+      <c r="AU62" s="22"/>
+      <c r="AV62" s="22"/>
+      <c r="AW62" s="22"/>
+      <c r="AX62" s="22"/>
+      <c r="AY62" s="22"/>
+      <c r="AZ62" s="22"/>
+      <c r="BA62" s="22"/>
+      <c r="BB62" s="22"/>
+      <c r="BC62" s="22"/>
+      <c r="BD62" s="22"/>
+      <c r="BE62" s="22"/>
+      <c r="BF62" s="22"/>
+      <c r="BG62" s="22"/>
+      <c r="BH62" s="22"/>
+      <c r="BI62" s="22"/>
+      <c r="BJ62" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="BK62" s="13"/>
-      <c r="BL62" s="13"/>
-      <c r="BM62" s="13"/>
-      <c r="BN62" s="13"/>
-      <c r="BO62" s="13"/>
-      <c r="BP62" s="13"/>
-      <c r="BQ62" s="13"/>
-      <c r="BR62" s="13"/>
-      <c r="BS62" s="13"/>
-      <c r="BT62" s="13"/>
-      <c r="BU62" s="13"/>
-      <c r="BV62" s="13"/>
-      <c r="BW62" s="13"/>
-      <c r="BX62" s="13"/>
-      <c r="BY62" s="13"/>
-      <c r="BZ62" s="13"/>
-      <c r="CA62" s="13"/>
-      <c r="CB62" s="13"/>
-      <c r="CC62" s="13"/>
-      <c r="CD62" s="13"/>
-      <c r="CE62" s="13"/>
-      <c r="CF62" s="13"/>
-      <c r="CG62" s="13"/>
-      <c r="CH62" s="13"/>
-      <c r="CI62" s="13"/>
-      <c r="CJ62" s="13"/>
-      <c r="CK62" s="13"/>
-      <c r="CL62" s="13"/>
-      <c r="CM62" s="13"/>
-      <c r="CN62" s="13"/>
-      <c r="CO62" s="13"/>
-      <c r="CP62" s="13"/>
-      <c r="CQ62" s="13"/>
-      <c r="CR62" s="13"/>
-      <c r="CS62" s="13"/>
-      <c r="CT62" s="15"/>
+      <c r="BK62" s="21"/>
+      <c r="BL62" s="21"/>
+      <c r="BM62" s="21"/>
+      <c r="BN62" s="21"/>
+      <c r="BO62" s="21"/>
+      <c r="BP62" s="21"/>
+      <c r="BQ62" s="21"/>
+      <c r="BR62" s="21"/>
+      <c r="BS62" s="21"/>
+      <c r="BT62" s="21"/>
+      <c r="BU62" s="21"/>
+      <c r="BV62" s="21"/>
+      <c r="BW62" s="21"/>
+      <c r="BX62" s="21"/>
+      <c r="BY62" s="21"/>
+      <c r="BZ62" s="21"/>
+      <c r="CA62" s="21"/>
+      <c r="CB62" s="21"/>
+      <c r="CC62" s="21"/>
+      <c r="CD62" s="21"/>
+      <c r="CE62" s="21"/>
+      <c r="CF62" s="21"/>
+      <c r="CG62" s="21"/>
+      <c r="CH62" s="21"/>
+      <c r="CI62" s="21"/>
+      <c r="CJ62" s="21"/>
+      <c r="CK62" s="21"/>
+      <c r="CL62" s="21"/>
+      <c r="CM62" s="21"/>
+      <c r="CN62" s="21"/>
+      <c r="CO62" s="21"/>
+      <c r="CP62" s="21"/>
+      <c r="CQ62" s="21"/>
+      <c r="CR62" s="21"/>
+      <c r="CS62" s="21"/>
+      <c r="CT62" s="23"/>
     </row>
     <row r="63" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C63" s="24">
+      <c r="C63" s="17">
         <v>3</v>
       </c>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="22" t="s">
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H63" s="22"/>
-      <c r="I63" s="22"/>
-      <c r="J63" s="22"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="22"/>
-      <c r="N63" s="22"/>
-      <c r="O63" s="22"/>
-      <c r="P63" s="22"/>
-      <c r="Q63" s="22"/>
-      <c r="R63" s="22"/>
-      <c r="S63" s="22"/>
-      <c r="T63" s="22"/>
-      <c r="U63" s="22"/>
-      <c r="V63" s="22"/>
-      <c r="W63" s="22"/>
-      <c r="X63" s="22"/>
-      <c r="Y63" s="22" t="s">
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13"/>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="R63" s="13"/>
+      <c r="S63" s="13"/>
+      <c r="T63" s="13"/>
+      <c r="U63" s="13"/>
+      <c r="V63" s="13"/>
+      <c r="W63" s="13"/>
+      <c r="X63" s="13"/>
+      <c r="Y63" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Z63" s="22"/>
-      <c r="AA63" s="22"/>
-      <c r="AB63" s="22"/>
-      <c r="AC63" s="22"/>
-      <c r="AD63" s="22"/>
-      <c r="AE63" s="22"/>
-      <c r="AF63" s="22"/>
-      <c r="AG63" s="22"/>
-      <c r="AH63" s="22"/>
-      <c r="AI63" s="22"/>
-      <c r="AJ63" s="22"/>
-      <c r="AK63" s="22"/>
-      <c r="AL63" s="22"/>
-      <c r="AM63" s="22"/>
-      <c r="AN63" s="25" t="s">
+      <c r="Z63" s="13"/>
+      <c r="AA63" s="13"/>
+      <c r="AB63" s="13"/>
+      <c r="AC63" s="13"/>
+      <c r="AD63" s="13"/>
+      <c r="AE63" s="13"/>
+      <c r="AF63" s="13"/>
+      <c r="AG63" s="13"/>
+      <c r="AH63" s="13"/>
+      <c r="AI63" s="13"/>
+      <c r="AJ63" s="13"/>
+      <c r="AK63" s="13"/>
+      <c r="AL63" s="13"/>
+      <c r="AM63" s="13"/>
+      <c r="AN63" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AO63" s="25"/>
-      <c r="AP63" s="25"/>
-      <c r="AQ63" s="25"/>
-      <c r="AR63" s="25"/>
-      <c r="AS63" s="25"/>
-      <c r="AT63" s="25"/>
-      <c r="AU63" s="25"/>
-      <c r="AV63" s="25"/>
-      <c r="AW63" s="25"/>
-      <c r="AX63" s="25"/>
-      <c r="AY63" s="25"/>
-      <c r="AZ63" s="25"/>
-      <c r="BA63" s="25"/>
-      <c r="BB63" s="25"/>
-      <c r="BC63" s="25"/>
-      <c r="BD63" s="25"/>
-      <c r="BE63" s="25"/>
-      <c r="BF63" s="25"/>
-      <c r="BG63" s="25"/>
-      <c r="BH63" s="25"/>
-      <c r="BI63" s="25"/>
-      <c r="BJ63" s="22"/>
-      <c r="BK63" s="22"/>
-      <c r="BL63" s="22"/>
-      <c r="BM63" s="22"/>
-      <c r="BN63" s="22"/>
-      <c r="BO63" s="22"/>
-      <c r="BP63" s="22"/>
-      <c r="BQ63" s="22"/>
-      <c r="BR63" s="22"/>
-      <c r="BS63" s="22"/>
-      <c r="BT63" s="22"/>
-      <c r="BU63" s="22"/>
-      <c r="BV63" s="22"/>
-      <c r="BW63" s="22"/>
-      <c r="BX63" s="22"/>
-      <c r="BY63" s="22"/>
-      <c r="BZ63" s="22"/>
-      <c r="CA63" s="22"/>
-      <c r="CB63" s="22"/>
-      <c r="CC63" s="22"/>
-      <c r="CD63" s="22"/>
-      <c r="CE63" s="22"/>
-      <c r="CF63" s="22"/>
-      <c r="CG63" s="22"/>
-      <c r="CH63" s="22"/>
-      <c r="CI63" s="22"/>
-      <c r="CJ63" s="22"/>
-      <c r="CK63" s="22"/>
-      <c r="CL63" s="22"/>
-      <c r="CM63" s="22"/>
-      <c r="CN63" s="22"/>
-      <c r="CO63" s="22"/>
-      <c r="CP63" s="22"/>
-      <c r="CQ63" s="22"/>
-      <c r="CR63" s="22"/>
-      <c r="CS63" s="22"/>
-      <c r="CT63" s="23"/>
+      <c r="AO63" s="18"/>
+      <c r="AP63" s="18"/>
+      <c r="AQ63" s="18"/>
+      <c r="AR63" s="18"/>
+      <c r="AS63" s="18"/>
+      <c r="AT63" s="18"/>
+      <c r="AU63" s="18"/>
+      <c r="AV63" s="18"/>
+      <c r="AW63" s="18"/>
+      <c r="AX63" s="18"/>
+      <c r="AY63" s="18"/>
+      <c r="AZ63" s="18"/>
+      <c r="BA63" s="18"/>
+      <c r="BB63" s="18"/>
+      <c r="BC63" s="18"/>
+      <c r="BD63" s="18"/>
+      <c r="BE63" s="18"/>
+      <c r="BF63" s="18"/>
+      <c r="BG63" s="18"/>
+      <c r="BH63" s="18"/>
+      <c r="BI63" s="18"/>
+      <c r="BJ63" s="13"/>
+      <c r="BK63" s="13"/>
+      <c r="BL63" s="13"/>
+      <c r="BM63" s="13"/>
+      <c r="BN63" s="13"/>
+      <c r="BO63" s="13"/>
+      <c r="BP63" s="13"/>
+      <c r="BQ63" s="13"/>
+      <c r="BR63" s="13"/>
+      <c r="BS63" s="13"/>
+      <c r="BT63" s="13"/>
+      <c r="BU63" s="13"/>
+      <c r="BV63" s="13"/>
+      <c r="BW63" s="13"/>
+      <c r="BX63" s="13"/>
+      <c r="BY63" s="13"/>
+      <c r="BZ63" s="13"/>
+      <c r="CA63" s="13"/>
+      <c r="CB63" s="13"/>
+      <c r="CC63" s="13"/>
+      <c r="CD63" s="13"/>
+      <c r="CE63" s="13"/>
+      <c r="CF63" s="13"/>
+      <c r="CG63" s="13"/>
+      <c r="CH63" s="13"/>
+      <c r="CI63" s="13"/>
+      <c r="CJ63" s="13"/>
+      <c r="CK63" s="13"/>
+      <c r="CL63" s="13"/>
+      <c r="CM63" s="13"/>
+      <c r="CN63" s="13"/>
+      <c r="CO63" s="13"/>
+      <c r="CP63" s="13"/>
+      <c r="CQ63" s="13"/>
+      <c r="CR63" s="13"/>
+      <c r="CS63" s="13"/>
+      <c r="CT63" s="14"/>
     </row>
     <row r="64" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C64" s="24">
+      <c r="C64" s="17">
         <v>4</v>
       </c>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="Y64" s="22"/>
-      <c r="Z64" s="22"/>
-      <c r="AA64" s="22"/>
-      <c r="AB64" s="22"/>
-      <c r="AC64" s="22"/>
-      <c r="AD64" s="22"/>
-      <c r="AE64" s="22"/>
-      <c r="AF64" s="22"/>
-      <c r="AG64" s="22"/>
-      <c r="AH64" s="22"/>
-      <c r="AI64" s="22"/>
-      <c r="AJ64" s="22"/>
-      <c r="AK64" s="22"/>
-      <c r="AL64" s="22"/>
-      <c r="AM64" s="22"/>
-      <c r="AN64" s="25"/>
-      <c r="AO64" s="25"/>
-      <c r="AP64" s="25"/>
-      <c r="AQ64" s="25"/>
-      <c r="AR64" s="25"/>
-      <c r="AS64" s="25"/>
-      <c r="AT64" s="25"/>
-      <c r="AU64" s="25"/>
-      <c r="AV64" s="25"/>
-      <c r="AW64" s="25"/>
-      <c r="AX64" s="25"/>
-      <c r="AY64" s="25"/>
-      <c r="AZ64" s="25"/>
-      <c r="BA64" s="25"/>
-      <c r="BB64" s="25"/>
-      <c r="BC64" s="25"/>
-      <c r="BD64" s="25"/>
-      <c r="BE64" s="25"/>
-      <c r="BF64" s="25"/>
-      <c r="BG64" s="25"/>
-      <c r="BH64" s="25"/>
-      <c r="BI64" s="25"/>
-      <c r="BJ64" s="22"/>
-      <c r="BK64" s="22"/>
-      <c r="BL64" s="22"/>
-      <c r="BM64" s="22"/>
-      <c r="BN64" s="22"/>
-      <c r="BO64" s="22"/>
-      <c r="BP64" s="22"/>
-      <c r="BQ64" s="22"/>
-      <c r="BR64" s="22"/>
-      <c r="BS64" s="22"/>
-      <c r="BT64" s="22"/>
-      <c r="BU64" s="22"/>
-      <c r="BV64" s="22"/>
-      <c r="BW64" s="22"/>
-      <c r="BX64" s="22"/>
-      <c r="BY64" s="22"/>
-      <c r="BZ64" s="22"/>
-      <c r="CA64" s="22"/>
-      <c r="CB64" s="22"/>
-      <c r="CC64" s="22"/>
-      <c r="CD64" s="22"/>
-      <c r="CE64" s="22"/>
-      <c r="CF64" s="22"/>
-      <c r="CG64" s="22"/>
-      <c r="CH64" s="22"/>
-      <c r="CI64" s="22"/>
-      <c r="CJ64" s="22"/>
-      <c r="CK64" s="22"/>
-      <c r="CL64" s="22"/>
-      <c r="CM64" s="22"/>
-      <c r="CN64" s="22"/>
-      <c r="CO64" s="22"/>
-      <c r="CP64" s="22"/>
-      <c r="CQ64" s="22"/>
-      <c r="CR64" s="22"/>
-      <c r="CS64" s="22"/>
-      <c r="CT64" s="23"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="Y64" s="13"/>
+      <c r="Z64" s="13"/>
+      <c r="AA64" s="13"/>
+      <c r="AB64" s="13"/>
+      <c r="AC64" s="13"/>
+      <c r="AD64" s="13"/>
+      <c r="AE64" s="13"/>
+      <c r="AF64" s="13"/>
+      <c r="AG64" s="13"/>
+      <c r="AH64" s="13"/>
+      <c r="AI64" s="13"/>
+      <c r="AJ64" s="13"/>
+      <c r="AK64" s="13"/>
+      <c r="AL64" s="13"/>
+      <c r="AM64" s="13"/>
+      <c r="AN64" s="18"/>
+      <c r="AO64" s="18"/>
+      <c r="AP64" s="18"/>
+      <c r="AQ64" s="18"/>
+      <c r="AR64" s="18"/>
+      <c r="AS64" s="18"/>
+      <c r="AT64" s="18"/>
+      <c r="AU64" s="18"/>
+      <c r="AV64" s="18"/>
+      <c r="AW64" s="18"/>
+      <c r="AX64" s="18"/>
+      <c r="AY64" s="18"/>
+      <c r="AZ64" s="18"/>
+      <c r="BA64" s="18"/>
+      <c r="BB64" s="18"/>
+      <c r="BC64" s="18"/>
+      <c r="BD64" s="18"/>
+      <c r="BE64" s="18"/>
+      <c r="BF64" s="18"/>
+      <c r="BG64" s="18"/>
+      <c r="BH64" s="18"/>
+      <c r="BI64" s="18"/>
+      <c r="BJ64" s="13"/>
+      <c r="BK64" s="13"/>
+      <c r="BL64" s="13"/>
+      <c r="BM64" s="13"/>
+      <c r="BN64" s="13"/>
+      <c r="BO64" s="13"/>
+      <c r="BP64" s="13"/>
+      <c r="BQ64" s="13"/>
+      <c r="BR64" s="13"/>
+      <c r="BS64" s="13"/>
+      <c r="BT64" s="13"/>
+      <c r="BU64" s="13"/>
+      <c r="BV64" s="13"/>
+      <c r="BW64" s="13"/>
+      <c r="BX64" s="13"/>
+      <c r="BY64" s="13"/>
+      <c r="BZ64" s="13"/>
+      <c r="CA64" s="13"/>
+      <c r="CB64" s="13"/>
+      <c r="CC64" s="13"/>
+      <c r="CD64" s="13"/>
+      <c r="CE64" s="13"/>
+      <c r="CF64" s="13"/>
+      <c r="CG64" s="13"/>
+      <c r="CH64" s="13"/>
+      <c r="CI64" s="13"/>
+      <c r="CJ64" s="13"/>
+      <c r="CK64" s="13"/>
+      <c r="CL64" s="13"/>
+      <c r="CM64" s="13"/>
+      <c r="CN64" s="13"/>
+      <c r="CO64" s="13"/>
+      <c r="CP64" s="13"/>
+      <c r="CQ64" s="13"/>
+      <c r="CR64" s="13"/>
+      <c r="CS64" s="13"/>
+      <c r="CT64" s="14"/>
     </row>
     <row r="65" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C65" s="24"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22"/>
-      <c r="I65" s="22"/>
-      <c r="J65" s="22"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="22"/>
-      <c r="N65" s="22"/>
-      <c r="O65" s="22"/>
-      <c r="P65" s="22"/>
-      <c r="Q65" s="22"/>
-      <c r="R65" s="22"/>
-      <c r="S65" s="22"/>
-      <c r="T65" s="22"/>
-      <c r="U65" s="22"/>
-      <c r="V65" s="22"/>
-      <c r="W65" s="22"/>
-      <c r="X65" s="22"/>
-      <c r="Y65" s="22"/>
-      <c r="Z65" s="22"/>
-      <c r="AA65" s="22"/>
-      <c r="AB65" s="22"/>
-      <c r="AC65" s="22"/>
-      <c r="AD65" s="22"/>
-      <c r="AE65" s="22"/>
-      <c r="AF65" s="22"/>
-      <c r="AG65" s="22"/>
-      <c r="AH65" s="22"/>
-      <c r="AI65" s="22"/>
-      <c r="AJ65" s="22"/>
-      <c r="AK65" s="22"/>
-      <c r="AL65" s="22"/>
-      <c r="AM65" s="22"/>
-      <c r="AN65" s="25"/>
-      <c r="AO65" s="25"/>
-      <c r="AP65" s="25"/>
-      <c r="AQ65" s="25"/>
-      <c r="AR65" s="25"/>
-      <c r="AS65" s="25"/>
-      <c r="AT65" s="25"/>
-      <c r="AU65" s="25"/>
-      <c r="AV65" s="25"/>
-      <c r="AW65" s="25"/>
-      <c r="AX65" s="25"/>
-      <c r="AY65" s="25"/>
-      <c r="AZ65" s="25"/>
-      <c r="BA65" s="25"/>
-      <c r="BB65" s="25"/>
-      <c r="BC65" s="25"/>
-      <c r="BD65" s="25"/>
-      <c r="BE65" s="25"/>
-      <c r="BF65" s="25"/>
-      <c r="BG65" s="25"/>
-      <c r="BH65" s="25"/>
-      <c r="BI65" s="25"/>
-      <c r="BJ65" s="22"/>
-      <c r="BK65" s="22"/>
-      <c r="BL65" s="22"/>
-      <c r="BM65" s="22"/>
-      <c r="BN65" s="22"/>
-      <c r="BO65" s="22"/>
-      <c r="BP65" s="22"/>
-      <c r="BQ65" s="22"/>
-      <c r="BR65" s="22"/>
-      <c r="BS65" s="22"/>
-      <c r="BT65" s="22"/>
-      <c r="BU65" s="22"/>
-      <c r="BV65" s="22"/>
-      <c r="BW65" s="22"/>
-      <c r="BX65" s="22"/>
-      <c r="BY65" s="22"/>
-      <c r="BZ65" s="22"/>
-      <c r="CA65" s="22"/>
-      <c r="CB65" s="22"/>
-      <c r="CC65" s="22"/>
-      <c r="CD65" s="22"/>
-      <c r="CE65" s="22"/>
-      <c r="CF65" s="22"/>
-      <c r="CG65" s="22"/>
-      <c r="CH65" s="22"/>
-      <c r="CI65" s="22"/>
-      <c r="CJ65" s="22"/>
-      <c r="CK65" s="22"/>
-      <c r="CL65" s="22"/>
-      <c r="CM65" s="22"/>
-      <c r="CN65" s="22"/>
-      <c r="CO65" s="22"/>
-      <c r="CP65" s="22"/>
-      <c r="CQ65" s="22"/>
-      <c r="CR65" s="22"/>
-      <c r="CS65" s="22"/>
-      <c r="CT65" s="23"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
+      <c r="S65" s="13"/>
+      <c r="T65" s="13"/>
+      <c r="U65" s="13"/>
+      <c r="V65" s="13"/>
+      <c r="W65" s="13"/>
+      <c r="X65" s="13"/>
+      <c r="Y65" s="13"/>
+      <c r="Z65" s="13"/>
+      <c r="AA65" s="13"/>
+      <c r="AB65" s="13"/>
+      <c r="AC65" s="13"/>
+      <c r="AD65" s="13"/>
+      <c r="AE65" s="13"/>
+      <c r="AF65" s="13"/>
+      <c r="AG65" s="13"/>
+      <c r="AH65" s="13"/>
+      <c r="AI65" s="13"/>
+      <c r="AJ65" s="13"/>
+      <c r="AK65" s="13"/>
+      <c r="AL65" s="13"/>
+      <c r="AM65" s="13"/>
+      <c r="AN65" s="18"/>
+      <c r="AO65" s="18"/>
+      <c r="AP65" s="18"/>
+      <c r="AQ65" s="18"/>
+      <c r="AR65" s="18"/>
+      <c r="AS65" s="18"/>
+      <c r="AT65" s="18"/>
+      <c r="AU65" s="18"/>
+      <c r="AV65" s="18"/>
+      <c r="AW65" s="18"/>
+      <c r="AX65" s="18"/>
+      <c r="AY65" s="18"/>
+      <c r="AZ65" s="18"/>
+      <c r="BA65" s="18"/>
+      <c r="BB65" s="18"/>
+      <c r="BC65" s="18"/>
+      <c r="BD65" s="18"/>
+      <c r="BE65" s="18"/>
+      <c r="BF65" s="18"/>
+      <c r="BG65" s="18"/>
+      <c r="BH65" s="18"/>
+      <c r="BI65" s="18"/>
+      <c r="BJ65" s="13"/>
+      <c r="BK65" s="13"/>
+      <c r="BL65" s="13"/>
+      <c r="BM65" s="13"/>
+      <c r="BN65" s="13"/>
+      <c r="BO65" s="13"/>
+      <c r="BP65" s="13"/>
+      <c r="BQ65" s="13"/>
+      <c r="BR65" s="13"/>
+      <c r="BS65" s="13"/>
+      <c r="BT65" s="13"/>
+      <c r="BU65" s="13"/>
+      <c r="BV65" s="13"/>
+      <c r="BW65" s="13"/>
+      <c r="BX65" s="13"/>
+      <c r="BY65" s="13"/>
+      <c r="BZ65" s="13"/>
+      <c r="CA65" s="13"/>
+      <c r="CB65" s="13"/>
+      <c r="CC65" s="13"/>
+      <c r="CD65" s="13"/>
+      <c r="CE65" s="13"/>
+      <c r="CF65" s="13"/>
+      <c r="CG65" s="13"/>
+      <c r="CH65" s="13"/>
+      <c r="CI65" s="13"/>
+      <c r="CJ65" s="13"/>
+      <c r="CK65" s="13"/>
+      <c r="CL65" s="13"/>
+      <c r="CM65" s="13"/>
+      <c r="CN65" s="13"/>
+      <c r="CO65" s="13"/>
+      <c r="CP65" s="13"/>
+      <c r="CQ65" s="13"/>
+      <c r="CR65" s="13"/>
+      <c r="CS65" s="13"/>
+      <c r="CT65" s="14"/>
     </row>
     <row r="66" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="24"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="22"/>
-      <c r="H66" s="22"/>
-      <c r="I66" s="22"/>
-      <c r="J66" s="22"/>
-      <c r="K66" s="22"/>
-      <c r="L66" s="22"/>
-      <c r="M66" s="22"/>
-      <c r="N66" s="22"/>
-      <c r="O66" s="22"/>
-      <c r="P66" s="22"/>
-      <c r="Q66" s="22"/>
-      <c r="R66" s="22"/>
-      <c r="S66" s="22"/>
-      <c r="T66" s="22"/>
-      <c r="U66" s="22"/>
-      <c r="V66" s="22"/>
-      <c r="W66" s="22"/>
-      <c r="X66" s="22"/>
-      <c r="Y66" s="22"/>
-      <c r="Z66" s="22"/>
-      <c r="AA66" s="22"/>
-      <c r="AB66" s="22"/>
-      <c r="AC66" s="22"/>
-      <c r="AD66" s="22"/>
-      <c r="AE66" s="22"/>
-      <c r="AF66" s="22"/>
-      <c r="AG66" s="22"/>
-      <c r="AH66" s="22"/>
-      <c r="AI66" s="22"/>
-      <c r="AJ66" s="22"/>
-      <c r="AK66" s="22"/>
-      <c r="AL66" s="22"/>
-      <c r="AM66" s="22"/>
-      <c r="AN66" s="25"/>
-      <c r="AO66" s="25"/>
-      <c r="AP66" s="25"/>
-      <c r="AQ66" s="25"/>
-      <c r="AR66" s="25"/>
-      <c r="AS66" s="25"/>
-      <c r="AT66" s="25"/>
-      <c r="AU66" s="25"/>
-      <c r="AV66" s="25"/>
-      <c r="AW66" s="25"/>
-      <c r="AX66" s="25"/>
-      <c r="AY66" s="25"/>
-      <c r="AZ66" s="25"/>
-      <c r="BA66" s="25"/>
-      <c r="BB66" s="25"/>
-      <c r="BC66" s="25"/>
-      <c r="BD66" s="25"/>
-      <c r="BE66" s="25"/>
-      <c r="BF66" s="25"/>
-      <c r="BG66" s="25"/>
-      <c r="BH66" s="25"/>
-      <c r="BI66" s="25"/>
-      <c r="BJ66" s="22"/>
-      <c r="BK66" s="22"/>
-      <c r="BL66" s="22"/>
-      <c r="BM66" s="22"/>
-      <c r="BN66" s="22"/>
-      <c r="BO66" s="22"/>
-      <c r="BP66" s="22"/>
-      <c r="BQ66" s="22"/>
-      <c r="BR66" s="22"/>
-      <c r="BS66" s="22"/>
-      <c r="BT66" s="22"/>
-      <c r="BU66" s="22"/>
-      <c r="BV66" s="22"/>
-      <c r="BW66" s="22"/>
-      <c r="BX66" s="22"/>
-      <c r="BY66" s="22"/>
-      <c r="BZ66" s="22"/>
-      <c r="CA66" s="22"/>
-      <c r="CB66" s="22"/>
-      <c r="CC66" s="22"/>
-      <c r="CD66" s="22"/>
-      <c r="CE66" s="22"/>
-      <c r="CF66" s="22"/>
-      <c r="CG66" s="22"/>
-      <c r="CH66" s="22"/>
-      <c r="CI66" s="22"/>
-      <c r="CJ66" s="22"/>
-      <c r="CK66" s="22"/>
-      <c r="CL66" s="22"/>
-      <c r="CM66" s="22"/>
-      <c r="CN66" s="22"/>
-      <c r="CO66" s="22"/>
-      <c r="CP66" s="22"/>
-      <c r="CQ66" s="22"/>
-      <c r="CR66" s="22"/>
-      <c r="CS66" s="22"/>
-      <c r="CT66" s="23"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="13"/>
+      <c r="O66" s="13"/>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="13"/>
+      <c r="S66" s="13"/>
+      <c r="T66" s="13"/>
+      <c r="U66" s="13"/>
+      <c r="V66" s="13"/>
+      <c r="W66" s="13"/>
+      <c r="X66" s="13"/>
+      <c r="Y66" s="13"/>
+      <c r="Z66" s="13"/>
+      <c r="AA66" s="13"/>
+      <c r="AB66" s="13"/>
+      <c r="AC66" s="13"/>
+      <c r="AD66" s="13"/>
+      <c r="AE66" s="13"/>
+      <c r="AF66" s="13"/>
+      <c r="AG66" s="13"/>
+      <c r="AH66" s="13"/>
+      <c r="AI66" s="13"/>
+      <c r="AJ66" s="13"/>
+      <c r="AK66" s="13"/>
+      <c r="AL66" s="13"/>
+      <c r="AM66" s="13"/>
+      <c r="AN66" s="18"/>
+      <c r="AO66" s="18"/>
+      <c r="AP66" s="18"/>
+      <c r="AQ66" s="18"/>
+      <c r="AR66" s="18"/>
+      <c r="AS66" s="18"/>
+      <c r="AT66" s="18"/>
+      <c r="AU66" s="18"/>
+      <c r="AV66" s="18"/>
+      <c r="AW66" s="18"/>
+      <c r="AX66" s="18"/>
+      <c r="AY66" s="18"/>
+      <c r="AZ66" s="18"/>
+      <c r="BA66" s="18"/>
+      <c r="BB66" s="18"/>
+      <c r="BC66" s="18"/>
+      <c r="BD66" s="18"/>
+      <c r="BE66" s="18"/>
+      <c r="BF66" s="18"/>
+      <c r="BG66" s="18"/>
+      <c r="BH66" s="18"/>
+      <c r="BI66" s="18"/>
+      <c r="BJ66" s="13"/>
+      <c r="BK66" s="13"/>
+      <c r="BL66" s="13"/>
+      <c r="BM66" s="13"/>
+      <c r="BN66" s="13"/>
+      <c r="BO66" s="13"/>
+      <c r="BP66" s="13"/>
+      <c r="BQ66" s="13"/>
+      <c r="BR66" s="13"/>
+      <c r="BS66" s="13"/>
+      <c r="BT66" s="13"/>
+      <c r="BU66" s="13"/>
+      <c r="BV66" s="13"/>
+      <c r="BW66" s="13"/>
+      <c r="BX66" s="13"/>
+      <c r="BY66" s="13"/>
+      <c r="BZ66" s="13"/>
+      <c r="CA66" s="13"/>
+      <c r="CB66" s="13"/>
+      <c r="CC66" s="13"/>
+      <c r="CD66" s="13"/>
+      <c r="CE66" s="13"/>
+      <c r="CF66" s="13"/>
+      <c r="CG66" s="13"/>
+      <c r="CH66" s="13"/>
+      <c r="CI66" s="13"/>
+      <c r="CJ66" s="13"/>
+      <c r="CK66" s="13"/>
+      <c r="CL66" s="13"/>
+      <c r="CM66" s="13"/>
+      <c r="CN66" s="13"/>
+      <c r="CO66" s="13"/>
+      <c r="CP66" s="13"/>
+      <c r="CQ66" s="13"/>
+      <c r="CR66" s="13"/>
+      <c r="CS66" s="13"/>
+      <c r="CT66" s="14"/>
     </row>
     <row r="67" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="24"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="22"/>
-      <c r="H67" s="22"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="22"/>
-      <c r="K67" s="22"/>
-      <c r="L67" s="22"/>
-      <c r="M67" s="22"/>
-      <c r="N67" s="22"/>
-      <c r="O67" s="22"/>
-      <c r="P67" s="22"/>
-      <c r="Q67" s="22"/>
-      <c r="R67" s="22"/>
-      <c r="S67" s="22"/>
-      <c r="T67" s="22"/>
-      <c r="U67" s="22"/>
-      <c r="V67" s="22"/>
-      <c r="W67" s="22"/>
-      <c r="X67" s="22"/>
-      <c r="Y67" s="22"/>
-      <c r="Z67" s="22"/>
-      <c r="AA67" s="22"/>
-      <c r="AB67" s="22"/>
-      <c r="AC67" s="22"/>
-      <c r="AD67" s="22"/>
-      <c r="AE67" s="22"/>
-      <c r="AF67" s="22"/>
-      <c r="AG67" s="22"/>
-      <c r="AH67" s="22"/>
-      <c r="AI67" s="22"/>
-      <c r="AJ67" s="22"/>
-      <c r="AK67" s="22"/>
-      <c r="AL67" s="22"/>
-      <c r="AM67" s="22"/>
-      <c r="AN67" s="25"/>
-      <c r="AO67" s="25"/>
-      <c r="AP67" s="25"/>
-      <c r="AQ67" s="25"/>
-      <c r="AR67" s="25"/>
-      <c r="AS67" s="25"/>
-      <c r="AT67" s="25"/>
-      <c r="AU67" s="25"/>
-      <c r="AV67" s="25"/>
-      <c r="AW67" s="25"/>
-      <c r="AX67" s="25"/>
-      <c r="AY67" s="25"/>
-      <c r="AZ67" s="25"/>
-      <c r="BA67" s="25"/>
-      <c r="BB67" s="25"/>
-      <c r="BC67" s="25"/>
-      <c r="BD67" s="25"/>
-      <c r="BE67" s="25"/>
-      <c r="BF67" s="25"/>
-      <c r="BG67" s="25"/>
-      <c r="BH67" s="25"/>
-      <c r="BI67" s="25"/>
-      <c r="BJ67" s="22"/>
-      <c r="BK67" s="22"/>
-      <c r="BL67" s="22"/>
-      <c r="BM67" s="22"/>
-      <c r="BN67" s="22"/>
-      <c r="BO67" s="22"/>
-      <c r="BP67" s="22"/>
-      <c r="BQ67" s="22"/>
-      <c r="BR67" s="22"/>
-      <c r="BS67" s="22"/>
-      <c r="BT67" s="22"/>
-      <c r="BU67" s="22"/>
-      <c r="BV67" s="22"/>
-      <c r="BW67" s="22"/>
-      <c r="BX67" s="22"/>
-      <c r="BY67" s="22"/>
-      <c r="BZ67" s="22"/>
-      <c r="CA67" s="22"/>
-      <c r="CB67" s="22"/>
-      <c r="CC67" s="22"/>
-      <c r="CD67" s="22"/>
-      <c r="CE67" s="22"/>
-      <c r="CF67" s="22"/>
-      <c r="CG67" s="22"/>
-      <c r="CH67" s="22"/>
-      <c r="CI67" s="22"/>
-      <c r="CJ67" s="22"/>
-      <c r="CK67" s="22"/>
-      <c r="CL67" s="22"/>
-      <c r="CM67" s="22"/>
-      <c r="CN67" s="22"/>
-      <c r="CO67" s="22"/>
-      <c r="CP67" s="22"/>
-      <c r="CQ67" s="22"/>
-      <c r="CR67" s="22"/>
-      <c r="CS67" s="22"/>
-      <c r="CT67" s="23"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13"/>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="13"/>
+      <c r="S67" s="13"/>
+      <c r="T67" s="13"/>
+      <c r="U67" s="13"/>
+      <c r="V67" s="13"/>
+      <c r="W67" s="13"/>
+      <c r="X67" s="13"/>
+      <c r="Y67" s="13"/>
+      <c r="Z67" s="13"/>
+      <c r="AA67" s="13"/>
+      <c r="AB67" s="13"/>
+      <c r="AC67" s="13"/>
+      <c r="AD67" s="13"/>
+      <c r="AE67" s="13"/>
+      <c r="AF67" s="13"/>
+      <c r="AG67" s="13"/>
+      <c r="AH67" s="13"/>
+      <c r="AI67" s="13"/>
+      <c r="AJ67" s="13"/>
+      <c r="AK67" s="13"/>
+      <c r="AL67" s="13"/>
+      <c r="AM67" s="13"/>
+      <c r="AN67" s="18"/>
+      <c r="AO67" s="18"/>
+      <c r="AP67" s="18"/>
+      <c r="AQ67" s="18"/>
+      <c r="AR67" s="18"/>
+      <c r="AS67" s="18"/>
+      <c r="AT67" s="18"/>
+      <c r="AU67" s="18"/>
+      <c r="AV67" s="18"/>
+      <c r="AW67" s="18"/>
+      <c r="AX67" s="18"/>
+      <c r="AY67" s="18"/>
+      <c r="AZ67" s="18"/>
+      <c r="BA67" s="18"/>
+      <c r="BB67" s="18"/>
+      <c r="BC67" s="18"/>
+      <c r="BD67" s="18"/>
+      <c r="BE67" s="18"/>
+      <c r="BF67" s="18"/>
+      <c r="BG67" s="18"/>
+      <c r="BH67" s="18"/>
+      <c r="BI67" s="18"/>
+      <c r="BJ67" s="13"/>
+      <c r="BK67" s="13"/>
+      <c r="BL67" s="13"/>
+      <c r="BM67" s="13"/>
+      <c r="BN67" s="13"/>
+      <c r="BO67" s="13"/>
+      <c r="BP67" s="13"/>
+      <c r="BQ67" s="13"/>
+      <c r="BR67" s="13"/>
+      <c r="BS67" s="13"/>
+      <c r="BT67" s="13"/>
+      <c r="BU67" s="13"/>
+      <c r="BV67" s="13"/>
+      <c r="BW67" s="13"/>
+      <c r="BX67" s="13"/>
+      <c r="BY67" s="13"/>
+      <c r="BZ67" s="13"/>
+      <c r="CA67" s="13"/>
+      <c r="CB67" s="13"/>
+      <c r="CC67" s="13"/>
+      <c r="CD67" s="13"/>
+      <c r="CE67" s="13"/>
+      <c r="CF67" s="13"/>
+      <c r="CG67" s="13"/>
+      <c r="CH67" s="13"/>
+      <c r="CI67" s="13"/>
+      <c r="CJ67" s="13"/>
+      <c r="CK67" s="13"/>
+      <c r="CL67" s="13"/>
+      <c r="CM67" s="13"/>
+      <c r="CN67" s="13"/>
+      <c r="CO67" s="13"/>
+      <c r="CP67" s="13"/>
+      <c r="CQ67" s="13"/>
+      <c r="CR67" s="13"/>
+      <c r="CS67" s="13"/>
+      <c r="CT67" s="14"/>
     </row>
     <row r="68" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="24"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="22"/>
-      <c r="H68" s="22"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="22"/>
-      <c r="K68" s="22"/>
-      <c r="L68" s="22"/>
-      <c r="M68" s="22"/>
-      <c r="N68" s="22"/>
-      <c r="O68" s="22"/>
-      <c r="P68" s="22"/>
-      <c r="Q68" s="22"/>
-      <c r="R68" s="22"/>
-      <c r="S68" s="22"/>
-      <c r="T68" s="22"/>
-      <c r="U68" s="22"/>
-      <c r="V68" s="22"/>
-      <c r="W68" s="22"/>
-      <c r="X68" s="22"/>
-      <c r="Y68" s="22"/>
-      <c r="Z68" s="22"/>
-      <c r="AA68" s="22"/>
-      <c r="AB68" s="22"/>
-      <c r="AC68" s="22"/>
-      <c r="AD68" s="22"/>
-      <c r="AE68" s="22"/>
-      <c r="AF68" s="22"/>
-      <c r="AG68" s="22"/>
-      <c r="AH68" s="22"/>
-      <c r="AI68" s="22"/>
-      <c r="AJ68" s="22"/>
-      <c r="AK68" s="22"/>
-      <c r="AL68" s="22"/>
-      <c r="AM68" s="22"/>
-      <c r="AN68" s="25"/>
-      <c r="AO68" s="25"/>
-      <c r="AP68" s="25"/>
-      <c r="AQ68" s="25"/>
-      <c r="AR68" s="25"/>
-      <c r="AS68" s="25"/>
-      <c r="AT68" s="25"/>
-      <c r="AU68" s="25"/>
-      <c r="AV68" s="25"/>
-      <c r="AW68" s="25"/>
-      <c r="AX68" s="25"/>
-      <c r="AY68" s="25"/>
-      <c r="AZ68" s="25"/>
-      <c r="BA68" s="25"/>
-      <c r="BB68" s="25"/>
-      <c r="BC68" s="25"/>
-      <c r="BD68" s="25"/>
-      <c r="BE68" s="25"/>
-      <c r="BF68" s="25"/>
-      <c r="BG68" s="25"/>
-      <c r="BH68" s="25"/>
-      <c r="BI68" s="25"/>
-      <c r="BJ68" s="22"/>
-      <c r="BK68" s="22"/>
-      <c r="BL68" s="22"/>
-      <c r="BM68" s="22"/>
-      <c r="BN68" s="22"/>
-      <c r="BO68" s="22"/>
-      <c r="BP68" s="22"/>
-      <c r="BQ68" s="22"/>
-      <c r="BR68" s="22"/>
-      <c r="BS68" s="22"/>
-      <c r="BT68" s="22"/>
-      <c r="BU68" s="22"/>
-      <c r="BV68" s="22"/>
-      <c r="BW68" s="22"/>
-      <c r="BX68" s="22"/>
-      <c r="BY68" s="22"/>
-      <c r="BZ68" s="22"/>
-      <c r="CA68" s="22"/>
-      <c r="CB68" s="22"/>
-      <c r="CC68" s="22"/>
-      <c r="CD68" s="22"/>
-      <c r="CE68" s="22"/>
-      <c r="CF68" s="22"/>
-      <c r="CG68" s="22"/>
-      <c r="CH68" s="22"/>
-      <c r="CI68" s="22"/>
-      <c r="CJ68" s="22"/>
-      <c r="CK68" s="22"/>
-      <c r="CL68" s="22"/>
-      <c r="CM68" s="22"/>
-      <c r="CN68" s="22"/>
-      <c r="CO68" s="22"/>
-      <c r="CP68" s="22"/>
-      <c r="CQ68" s="22"/>
-      <c r="CR68" s="22"/>
-      <c r="CS68" s="22"/>
-      <c r="CT68" s="23"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="13"/>
+      <c r="S68" s="13"/>
+      <c r="T68" s="13"/>
+      <c r="U68" s="13"/>
+      <c r="V68" s="13"/>
+      <c r="W68" s="13"/>
+      <c r="X68" s="13"/>
+      <c r="Y68" s="13"/>
+      <c r="Z68" s="13"/>
+      <c r="AA68" s="13"/>
+      <c r="AB68" s="13"/>
+      <c r="AC68" s="13"/>
+      <c r="AD68" s="13"/>
+      <c r="AE68" s="13"/>
+      <c r="AF68" s="13"/>
+      <c r="AG68" s="13"/>
+      <c r="AH68" s="13"/>
+      <c r="AI68" s="13"/>
+      <c r="AJ68" s="13"/>
+      <c r="AK68" s="13"/>
+      <c r="AL68" s="13"/>
+      <c r="AM68" s="13"/>
+      <c r="AN68" s="18"/>
+      <c r="AO68" s="18"/>
+      <c r="AP68" s="18"/>
+      <c r="AQ68" s="18"/>
+      <c r="AR68" s="18"/>
+      <c r="AS68" s="18"/>
+      <c r="AT68" s="18"/>
+      <c r="AU68" s="18"/>
+      <c r="AV68" s="18"/>
+      <c r="AW68" s="18"/>
+      <c r="AX68" s="18"/>
+      <c r="AY68" s="18"/>
+      <c r="AZ68" s="18"/>
+      <c r="BA68" s="18"/>
+      <c r="BB68" s="18"/>
+      <c r="BC68" s="18"/>
+      <c r="BD68" s="18"/>
+      <c r="BE68" s="18"/>
+      <c r="BF68" s="18"/>
+      <c r="BG68" s="18"/>
+      <c r="BH68" s="18"/>
+      <c r="BI68" s="18"/>
+      <c r="BJ68" s="13"/>
+      <c r="BK68" s="13"/>
+      <c r="BL68" s="13"/>
+      <c r="BM68" s="13"/>
+      <c r="BN68" s="13"/>
+      <c r="BO68" s="13"/>
+      <c r="BP68" s="13"/>
+      <c r="BQ68" s="13"/>
+      <c r="BR68" s="13"/>
+      <c r="BS68" s="13"/>
+      <c r="BT68" s="13"/>
+      <c r="BU68" s="13"/>
+      <c r="BV68" s="13"/>
+      <c r="BW68" s="13"/>
+      <c r="BX68" s="13"/>
+      <c r="BY68" s="13"/>
+      <c r="BZ68" s="13"/>
+      <c r="CA68" s="13"/>
+      <c r="CB68" s="13"/>
+      <c r="CC68" s="13"/>
+      <c r="CD68" s="13"/>
+      <c r="CE68" s="13"/>
+      <c r="CF68" s="13"/>
+      <c r="CG68" s="13"/>
+      <c r="CH68" s="13"/>
+      <c r="CI68" s="13"/>
+      <c r="CJ68" s="13"/>
+      <c r="CK68" s="13"/>
+      <c r="CL68" s="13"/>
+      <c r="CM68" s="13"/>
+      <c r="CN68" s="13"/>
+      <c r="CO68" s="13"/>
+      <c r="CP68" s="13"/>
+      <c r="CQ68" s="13"/>
+      <c r="CR68" s="13"/>
+      <c r="CS68" s="13"/>
+      <c r="CT68" s="14"/>
     </row>
     <row r="69" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C69" s="24"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="22"/>
-      <c r="H69" s="22"/>
-      <c r="I69" s="22"/>
-      <c r="J69" s="22"/>
-      <c r="K69" s="22"/>
-      <c r="L69" s="22"/>
-      <c r="M69" s="22"/>
-      <c r="N69" s="22"/>
-      <c r="O69" s="22"/>
-      <c r="P69" s="22"/>
-      <c r="Q69" s="22"/>
-      <c r="R69" s="22"/>
-      <c r="S69" s="22"/>
-      <c r="T69" s="22"/>
-      <c r="U69" s="22"/>
-      <c r="V69" s="22"/>
-      <c r="W69" s="22"/>
-      <c r="X69" s="22"/>
-      <c r="Y69" s="22"/>
-      <c r="Z69" s="22"/>
-      <c r="AA69" s="22"/>
-      <c r="AB69" s="22"/>
-      <c r="AC69" s="22"/>
-      <c r="AD69" s="22"/>
-      <c r="AE69" s="22"/>
-      <c r="AF69" s="22"/>
-      <c r="AG69" s="22"/>
-      <c r="AH69" s="22"/>
-      <c r="AI69" s="22"/>
-      <c r="AJ69" s="22"/>
-      <c r="AK69" s="22"/>
-      <c r="AL69" s="22"/>
-      <c r="AM69" s="22"/>
-      <c r="AN69" s="25"/>
-      <c r="AO69" s="25"/>
-      <c r="AP69" s="25"/>
-      <c r="AQ69" s="25"/>
-      <c r="AR69" s="25"/>
-      <c r="AS69" s="25"/>
-      <c r="AT69" s="25"/>
-      <c r="AU69" s="25"/>
-      <c r="AV69" s="25"/>
-      <c r="AW69" s="25"/>
-      <c r="AX69" s="25"/>
-      <c r="AY69" s="25"/>
-      <c r="AZ69" s="25"/>
-      <c r="BA69" s="25"/>
-      <c r="BB69" s="25"/>
-      <c r="BC69" s="25"/>
-      <c r="BD69" s="25"/>
-      <c r="BE69" s="25"/>
-      <c r="BF69" s="25"/>
-      <c r="BG69" s="25"/>
-      <c r="BH69" s="25"/>
-      <c r="BI69" s="25"/>
-      <c r="BJ69" s="22"/>
-      <c r="BK69" s="22"/>
-      <c r="BL69" s="22"/>
-      <c r="BM69" s="22"/>
-      <c r="BN69" s="22"/>
-      <c r="BO69" s="22"/>
-      <c r="BP69" s="22"/>
-      <c r="BQ69" s="22"/>
-      <c r="BR69" s="22"/>
-      <c r="BS69" s="22"/>
-      <c r="BT69" s="22"/>
-      <c r="BU69" s="22"/>
-      <c r="BV69" s="22"/>
-      <c r="BW69" s="22"/>
-      <c r="BX69" s="22"/>
-      <c r="BY69" s="22"/>
-      <c r="BZ69" s="22"/>
-      <c r="CA69" s="22"/>
-      <c r="CB69" s="22"/>
-      <c r="CC69" s="22"/>
-      <c r="CD69" s="22"/>
-      <c r="CE69" s="22"/>
-      <c r="CF69" s="22"/>
-      <c r="CG69" s="22"/>
-      <c r="CH69" s="22"/>
-      <c r="CI69" s="22"/>
-      <c r="CJ69" s="22"/>
-      <c r="CK69" s="22"/>
-      <c r="CL69" s="22"/>
-      <c r="CM69" s="22"/>
-      <c r="CN69" s="22"/>
-      <c r="CO69" s="22"/>
-      <c r="CP69" s="22"/>
-      <c r="CQ69" s="22"/>
-      <c r="CR69" s="22"/>
-      <c r="CS69" s="22"/>
-      <c r="CT69" s="23"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13"/>
+      <c r="O69" s="13"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="13"/>
+      <c r="S69" s="13"/>
+      <c r="T69" s="13"/>
+      <c r="U69" s="13"/>
+      <c r="V69" s="13"/>
+      <c r="W69" s="13"/>
+      <c r="X69" s="13"/>
+      <c r="Y69" s="13"/>
+      <c r="Z69" s="13"/>
+      <c r="AA69" s="13"/>
+      <c r="AB69" s="13"/>
+      <c r="AC69" s="13"/>
+      <c r="AD69" s="13"/>
+      <c r="AE69" s="13"/>
+      <c r="AF69" s="13"/>
+      <c r="AG69" s="13"/>
+      <c r="AH69" s="13"/>
+      <c r="AI69" s="13"/>
+      <c r="AJ69" s="13"/>
+      <c r="AK69" s="13"/>
+      <c r="AL69" s="13"/>
+      <c r="AM69" s="13"/>
+      <c r="AN69" s="18"/>
+      <c r="AO69" s="18"/>
+      <c r="AP69" s="18"/>
+      <c r="AQ69" s="18"/>
+      <c r="AR69" s="18"/>
+      <c r="AS69" s="18"/>
+      <c r="AT69" s="18"/>
+      <c r="AU69" s="18"/>
+      <c r="AV69" s="18"/>
+      <c r="AW69" s="18"/>
+      <c r="AX69" s="18"/>
+      <c r="AY69" s="18"/>
+      <c r="AZ69" s="18"/>
+      <c r="BA69" s="18"/>
+      <c r="BB69" s="18"/>
+      <c r="BC69" s="18"/>
+      <c r="BD69" s="18"/>
+      <c r="BE69" s="18"/>
+      <c r="BF69" s="18"/>
+      <c r="BG69" s="18"/>
+      <c r="BH69" s="18"/>
+      <c r="BI69" s="18"/>
+      <c r="BJ69" s="13"/>
+      <c r="BK69" s="13"/>
+      <c r="BL69" s="13"/>
+      <c r="BM69" s="13"/>
+      <c r="BN69" s="13"/>
+      <c r="BO69" s="13"/>
+      <c r="BP69" s="13"/>
+      <c r="BQ69" s="13"/>
+      <c r="BR69" s="13"/>
+      <c r="BS69" s="13"/>
+      <c r="BT69" s="13"/>
+      <c r="BU69" s="13"/>
+      <c r="BV69" s="13"/>
+      <c r="BW69" s="13"/>
+      <c r="BX69" s="13"/>
+      <c r="BY69" s="13"/>
+      <c r="BZ69" s="13"/>
+      <c r="CA69" s="13"/>
+      <c r="CB69" s="13"/>
+      <c r="CC69" s="13"/>
+      <c r="CD69" s="13"/>
+      <c r="CE69" s="13"/>
+      <c r="CF69" s="13"/>
+      <c r="CG69" s="13"/>
+      <c r="CH69" s="13"/>
+      <c r="CI69" s="13"/>
+      <c r="CJ69" s="13"/>
+      <c r="CK69" s="13"/>
+      <c r="CL69" s="13"/>
+      <c r="CM69" s="13"/>
+      <c r="CN69" s="13"/>
+      <c r="CO69" s="13"/>
+      <c r="CP69" s="13"/>
+      <c r="CQ69" s="13"/>
+      <c r="CR69" s="13"/>
+      <c r="CS69" s="13"/>
+      <c r="CT69" s="14"/>
     </row>
     <row r="70" spans="3:98" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="27"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="29"/>
-      <c r="I70" s="29"/>
-      <c r="J70" s="29"/>
-      <c r="K70" s="29"/>
-      <c r="L70" s="29"/>
-      <c r="M70" s="29"/>
-      <c r="N70" s="29"/>
-      <c r="O70" s="29"/>
-      <c r="P70" s="29"/>
-      <c r="Q70" s="29"/>
-      <c r="R70" s="29"/>
-      <c r="S70" s="29"/>
-      <c r="T70" s="29"/>
-      <c r="U70" s="29"/>
-      <c r="V70" s="29"/>
-      <c r="W70" s="29"/>
-      <c r="X70" s="29"/>
-      <c r="Y70" s="29"/>
-      <c r="Z70" s="29"/>
-      <c r="AA70" s="29"/>
-      <c r="AB70" s="29"/>
-      <c r="AC70" s="29"/>
-      <c r="AD70" s="29"/>
-      <c r="AE70" s="29"/>
-      <c r="AF70" s="29"/>
-      <c r="AG70" s="29"/>
-      <c r="AH70" s="29"/>
-      <c r="AI70" s="29"/>
-      <c r="AJ70" s="29"/>
-      <c r="AK70" s="29"/>
-      <c r="AL70" s="29"/>
-      <c r="AM70" s="29"/>
-      <c r="AN70" s="28"/>
-      <c r="AO70" s="28"/>
-      <c r="AP70" s="28"/>
-      <c r="AQ70" s="28"/>
-      <c r="AR70" s="28"/>
-      <c r="AS70" s="28"/>
-      <c r="AT70" s="28"/>
-      <c r="AU70" s="28"/>
-      <c r="AV70" s="28"/>
-      <c r="AW70" s="28"/>
-      <c r="AX70" s="28"/>
-      <c r="AY70" s="28"/>
-      <c r="AZ70" s="28"/>
-      <c r="BA70" s="28"/>
-      <c r="BB70" s="28"/>
-      <c r="BC70" s="28"/>
-      <c r="BD70" s="28"/>
-      <c r="BE70" s="28"/>
-      <c r="BF70" s="28"/>
-      <c r="BG70" s="28"/>
-      <c r="BH70" s="28"/>
-      <c r="BI70" s="28"/>
-      <c r="BJ70" s="29"/>
-      <c r="BK70" s="29"/>
-      <c r="BL70" s="29"/>
-      <c r="BM70" s="29"/>
-      <c r="BN70" s="29"/>
-      <c r="BO70" s="29"/>
-      <c r="BP70" s="29"/>
-      <c r="BQ70" s="29"/>
-      <c r="BR70" s="29"/>
-      <c r="BS70" s="29"/>
-      <c r="BT70" s="29"/>
-      <c r="BU70" s="29"/>
-      <c r="BV70" s="29"/>
-      <c r="BW70" s="29"/>
-      <c r="BX70" s="29"/>
-      <c r="BY70" s="29"/>
-      <c r="BZ70" s="29"/>
-      <c r="CA70" s="29"/>
-      <c r="CB70" s="29"/>
-      <c r="CC70" s="29"/>
-      <c r="CD70" s="29"/>
-      <c r="CE70" s="29"/>
-      <c r="CF70" s="29"/>
-      <c r="CG70" s="29"/>
-      <c r="CH70" s="29"/>
-      <c r="CI70" s="29"/>
-      <c r="CJ70" s="29"/>
-      <c r="CK70" s="29"/>
-      <c r="CL70" s="29"/>
-      <c r="CM70" s="29"/>
-      <c r="CN70" s="29"/>
-      <c r="CO70" s="29"/>
-      <c r="CP70" s="29"/>
-      <c r="CQ70" s="29"/>
-      <c r="CR70" s="29"/>
-      <c r="CS70" s="29"/>
-      <c r="CT70" s="30"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+      <c r="S70" s="15"/>
+      <c r="T70" s="15"/>
+      <c r="U70" s="15"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="15"/>
+      <c r="X70" s="15"/>
+      <c r="Y70" s="15"/>
+      <c r="Z70" s="15"/>
+      <c r="AA70" s="15"/>
+      <c r="AB70" s="15"/>
+      <c r="AC70" s="15"/>
+      <c r="AD70" s="15"/>
+      <c r="AE70" s="15"/>
+      <c r="AF70" s="15"/>
+      <c r="AG70" s="15"/>
+      <c r="AH70" s="15"/>
+      <c r="AI70" s="15"/>
+      <c r="AJ70" s="15"/>
+      <c r="AK70" s="15"/>
+      <c r="AL70" s="15"/>
+      <c r="AM70" s="15"/>
+      <c r="AN70" s="20"/>
+      <c r="AO70" s="20"/>
+      <c r="AP70" s="20"/>
+      <c r="AQ70" s="20"/>
+      <c r="AR70" s="20"/>
+      <c r="AS70" s="20"/>
+      <c r="AT70" s="20"/>
+      <c r="AU70" s="20"/>
+      <c r="AV70" s="20"/>
+      <c r="AW70" s="20"/>
+      <c r="AX70" s="20"/>
+      <c r="AY70" s="20"/>
+      <c r="AZ70" s="20"/>
+      <c r="BA70" s="20"/>
+      <c r="BB70" s="20"/>
+      <c r="BC70" s="20"/>
+      <c r="BD70" s="20"/>
+      <c r="BE70" s="20"/>
+      <c r="BF70" s="20"/>
+      <c r="BG70" s="20"/>
+      <c r="BH70" s="20"/>
+      <c r="BI70" s="20"/>
+      <c r="BJ70" s="15"/>
+      <c r="BK70" s="15"/>
+      <c r="BL70" s="15"/>
+      <c r="BM70" s="15"/>
+      <c r="BN70" s="15"/>
+      <c r="BO70" s="15"/>
+      <c r="BP70" s="15"/>
+      <c r="BQ70" s="15"/>
+      <c r="BR70" s="15"/>
+      <c r="BS70" s="15"/>
+      <c r="BT70" s="15"/>
+      <c r="BU70" s="15"/>
+      <c r="BV70" s="15"/>
+      <c r="BW70" s="15"/>
+      <c r="BX70" s="15"/>
+      <c r="BY70" s="15"/>
+      <c r="BZ70" s="15"/>
+      <c r="CA70" s="15"/>
+      <c r="CB70" s="15"/>
+      <c r="CC70" s="15"/>
+      <c r="CD70" s="15"/>
+      <c r="CE70" s="15"/>
+      <c r="CF70" s="15"/>
+      <c r="CG70" s="15"/>
+      <c r="CH70" s="15"/>
+      <c r="CI70" s="15"/>
+      <c r="CJ70" s="15"/>
+      <c r="CK70" s="15"/>
+      <c r="CL70" s="15"/>
+      <c r="CM70" s="15"/>
+      <c r="CN70" s="15"/>
+      <c r="CO70" s="15"/>
+      <c r="CP70" s="15"/>
+      <c r="CQ70" s="15"/>
+      <c r="CR70" s="15"/>
+      <c r="CS70" s="15"/>
+      <c r="CT70" s="16"/>
     </row>
     <row r="71" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="72" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7119,53 +7119,6 @@
     <row r="76" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="BZ65:CT65"/>
-    <mergeCell ref="BZ70:CT70"/>
-    <mergeCell ref="BZ69:CT69"/>
-    <mergeCell ref="BZ68:CT68"/>
-    <mergeCell ref="BZ67:CT67"/>
-    <mergeCell ref="BZ66:CT66"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="G69:X69"/>
-    <mergeCell ref="Y69:AM69"/>
-    <mergeCell ref="AN69:BI69"/>
-    <mergeCell ref="BJ69:BY69"/>
-    <mergeCell ref="C70:F70"/>
-    <mergeCell ref="G70:X70"/>
-    <mergeCell ref="Y70:AM70"/>
-    <mergeCell ref="AN70:BI70"/>
-    <mergeCell ref="BJ70:BY70"/>
-    <mergeCell ref="C67:F67"/>
-    <mergeCell ref="G67:X67"/>
-    <mergeCell ref="Y67:AM67"/>
-    <mergeCell ref="AN67:BI67"/>
-    <mergeCell ref="BJ67:BY67"/>
-    <mergeCell ref="C68:F68"/>
-    <mergeCell ref="G68:X68"/>
-    <mergeCell ref="Y68:AM68"/>
-    <mergeCell ref="AN68:BI68"/>
-    <mergeCell ref="BJ68:BY68"/>
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="G65:X65"/>
-    <mergeCell ref="Y65:AM65"/>
-    <mergeCell ref="AN65:BI65"/>
-    <mergeCell ref="BJ65:BY65"/>
-    <mergeCell ref="C66:F66"/>
-    <mergeCell ref="G66:X66"/>
-    <mergeCell ref="Y66:AM66"/>
-    <mergeCell ref="AN66:BI66"/>
-    <mergeCell ref="BJ66:BY66"/>
-    <mergeCell ref="BZ63:CT63"/>
-    <mergeCell ref="C63:F63"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="G63:X63"/>
-    <mergeCell ref="Y63:AM63"/>
-    <mergeCell ref="AN63:BI63"/>
-    <mergeCell ref="BJ63:BY63"/>
-    <mergeCell ref="Y64:AM64"/>
-    <mergeCell ref="AN64:BI64"/>
-    <mergeCell ref="BJ64:BY64"/>
-    <mergeCell ref="BZ64:CT64"/>
     <mergeCell ref="Y62:AM62"/>
     <mergeCell ref="AN62:BI62"/>
     <mergeCell ref="BZ62:CT62"/>
@@ -7182,6 +7135,53 @@
     <mergeCell ref="BJ62:BY62"/>
     <mergeCell ref="C62:F62"/>
     <mergeCell ref="G62:X62"/>
+    <mergeCell ref="BZ63:CT63"/>
+    <mergeCell ref="C63:F63"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="G63:X63"/>
+    <mergeCell ref="Y63:AM63"/>
+    <mergeCell ref="AN63:BI63"/>
+    <mergeCell ref="BJ63:BY63"/>
+    <mergeCell ref="Y64:AM64"/>
+    <mergeCell ref="AN64:BI64"/>
+    <mergeCell ref="BJ64:BY64"/>
+    <mergeCell ref="BZ64:CT64"/>
+    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="G66:X66"/>
+    <mergeCell ref="Y66:AM66"/>
+    <mergeCell ref="AN66:BI66"/>
+    <mergeCell ref="BJ66:BY66"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="G65:X65"/>
+    <mergeCell ref="Y65:AM65"/>
+    <mergeCell ref="AN65:BI65"/>
+    <mergeCell ref="BJ65:BY65"/>
+    <mergeCell ref="C68:F68"/>
+    <mergeCell ref="G68:X68"/>
+    <mergeCell ref="Y68:AM68"/>
+    <mergeCell ref="AN68:BI68"/>
+    <mergeCell ref="BJ68:BY68"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="G67:X67"/>
+    <mergeCell ref="Y67:AM67"/>
+    <mergeCell ref="AN67:BI67"/>
+    <mergeCell ref="BJ67:BY67"/>
+    <mergeCell ref="C70:F70"/>
+    <mergeCell ref="G70:X70"/>
+    <mergeCell ref="Y70:AM70"/>
+    <mergeCell ref="AN70:BI70"/>
+    <mergeCell ref="BJ70:BY70"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="G69:X69"/>
+    <mergeCell ref="Y69:AM69"/>
+    <mergeCell ref="AN69:BI69"/>
+    <mergeCell ref="BJ69:BY69"/>
+    <mergeCell ref="BZ65:CT65"/>
+    <mergeCell ref="BZ70:CT70"/>
+    <mergeCell ref="BZ69:CT69"/>
+    <mergeCell ref="BZ68:CT68"/>
+    <mergeCell ref="BZ67:CT67"/>
+    <mergeCell ref="BZ66:CT66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>